<commit_message>
Analysis excel file updated with the tables
Preprocess :
-Shuffle Param Added

SVM :
-GridSearch Function

CNN :
- MobileNetV2 Added
- class_weight
- f1 score
- optimizer param
</commit_message>
<xml_diff>
--- a/analysis/keras_results.xlsx
+++ b/analysis/keras_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t xml:space="preserve">CNN</t>
   </si>
@@ -74,6 +74,99 @@
   </si>
   <si>
     <t xml:space="preserve">smiling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smiling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNN no fc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNN+fc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neuron size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conv blocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dropoout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hidden Layers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epochs to converge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLP-dropout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNN3+fc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNN5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MobileNetV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Augment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Augmented Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slightly Augmented Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Augmented Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanced Class weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equal Class weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optimizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMSprop (0.0001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SGD (0.0001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam (0.0001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adagrad (0.0001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adadelta (0.0001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adamax (0.0001)</t>
   </si>
 </sst>
 </file>
@@ -150,7 +243,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,6 +272,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -196,21 +301,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K33" activeCellId="0" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.76530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8520408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,12 +491,15 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F14" s="0"/>
+      <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="0"/>
+      <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="0"/>
+      <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -399,6 +512,7 @@
       <c r="D17" s="5"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
+      <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -407,6 +521,12 @@
       <c r="B18" s="0" t="n">
         <v>0.75</v>
       </c>
+      <c r="F18" s="0"/>
+      <c r="I18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="0"/>
+      <c r="I19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -415,6 +535,8 @@
       <c r="B20" s="0" t="n">
         <v>0.296783088235</v>
       </c>
+      <c r="F20" s="0"/>
+      <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -423,6 +545,8 @@
       <c r="B21" s="0" t="n">
         <v>0.866544117647</v>
       </c>
+      <c r="F21" s="0"/>
+      <c r="I21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -431,6 +555,8 @@
       <c r="B22" s="0" t="n">
         <v>0.928860294118</v>
       </c>
+      <c r="F22" s="0"/>
+      <c r="I22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -439,6 +565,8 @@
       <c r="B23" s="0" t="n">
         <v>0.791176470588</v>
       </c>
+      <c r="F23" s="0"/>
+      <c r="I23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -447,10 +575,474 @@
       <c r="B24" s="0" t="n">
         <v>0.976470588235</v>
       </c>
+      <c r="F24" s="0"/>
+      <c r="I24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F25" s="0"/>
+      <c r="I25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F26" s="0"/>
+      <c r="I26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="0"/>
+      <c r="G27" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="0"/>
+      <c r="J27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="7"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="9" t="n">
+        <v>256</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L28" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F29" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F30" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="I30" s="0"/>
+      <c r="K30" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F31" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>0.293</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="I31" s="0"/>
+      <c r="K31" s="0" t="n">
+        <v>0.187</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F32" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>85.43</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="I32" s="0"/>
+      <c r="K32" s="0" t="n">
+        <v>92.88</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F33" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0.934</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>0.94</v>
+      </c>
+      <c r="I33" s="0"/>
+      <c r="K33" s="0" t="n">
+        <v>0.9571</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F34" s="0"/>
+      <c r="I34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F35" s="0"/>
+      <c r="I35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F36" s="0"/>
+      <c r="I36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F37" s="0"/>
+      <c r="I37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>27.93</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>85.97</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>88.16</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <v>0.8184</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>86.78</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>73.27</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>86.09</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>99.34</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <v>0.8313</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>91.03</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>85.43</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>90.8</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>92.88</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>0.8094</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>54.6</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>82.48</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>88.28</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>89.27</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <v>0.8674</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>97.82</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <v>99.12</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>99.12</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L43" s="0" t="n">
+        <v>0.9994</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F44" s="0"/>
+      <c r="I44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D45" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>81.82</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>90.69</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>81.93</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J46" s="0" t="n">
+        <v>92.88</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F47" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>91.03</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <v>88.5</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>90.8</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F48" s="0"/>
+      <c r="I48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D49" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>91.24</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <v>85.43</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>91.13</v>
+      </c>
+      <c r="J49" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F50" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>93.08</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>85.22</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>91.35</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F51" s="0"/>
+      <c r="I51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D52" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <v>81.93</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>81.9</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>92.88</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>85.43</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>90.8</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>81.93</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>89.27</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F55" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>82.36</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>87.51</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F56" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <v>84.23</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <v>88.17</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F57" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <v>81.93</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <v>81.93</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="K27:L27"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>